<commit_message>
- Sonar resolved 36 errors && added to report
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Scoala\Semestrul_6\Verificarea_si_validarea_sistemelor_soft\lab\lab\Verificare_si_validare_sisteme_soft\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08BE83E9-86CA-4129-84C3-7D795995A098}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD27BDBB-B95D-4703-9BBE-3EDAE47A3021}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="73">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -178,13 +178,476 @@
   </si>
   <si>
     <t>Da, factory</t>
+  </si>
+  <si>
+    <r>
+      <t>System.</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF9876AA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+      </rPr>
+      <t>out</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+      </rPr>
+      <t>.println(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+      </rPr>
+      <t>"Blank Fields"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ApplicationLogger.</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+      </rPr>
+      <t>log</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+      </rPr>
+      <t>(Level.</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF9876AA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+      </rPr>
+      <t>INFO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+      </rPr>
+      <t>"Blank Fields"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <t>ModifyPartController, 207</t>
+  </si>
+  <si>
+    <t>Standard outputs should not be used directly to log anything</t>
+  </si>
+  <si>
+    <t>Optional value should only be accessed after calling isPresent()</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">if </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">(result.get() </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+      </rPr>
+      <t>...</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">if </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+      </rPr>
+      <t>(result.isPresent() &amp;&amp; result.get()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve"> ...</t>
+    </r>
+  </si>
+  <si>
+    <t>Popa Cristi - Ionel</t>
+  </si>
+  <si>
+    <t>ModifyProductController, 175</t>
+  </si>
+  <si>
+    <t>Sections of code should not be commented out</t>
+  </si>
+  <si>
+    <t>//scene = FXMLLoader.load(getClass().getResource(source));</t>
+  </si>
+  <si>
+    <t>(blank)</t>
+  </si>
+  <si>
+    <t>ModifyPartController, 120</t>
+  </si>
+  <si>
+    <t>Constructors should not be used to instantiate "String", "BigInteger", "BigDecimal" and primitive-wrapper classes</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">private </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">String </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF9876AA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">errorMessage </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">= </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">new </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+      </rPr>
+      <t>String()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">private </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">String </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF9876AA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+      </rPr>
+      <t>errorMessage</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <t>ModifyPartController, 34</t>
+  </si>
+  <si>
+    <t>Unused "private" fields should be removed</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">private int </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF9876AA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+      </rPr>
+      <t>partId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <t>Methods should not be empty</t>
+  </si>
+  <si>
+    <t>ModifyPartController, 37</t>
+  </si>
+  <si>
+    <t>ModifyPartController, 69</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">public </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFFC66D"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+      </rPr>
+      <t>ModifyPartController</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+      </rPr>
+      <t>(){}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">public </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFFC66D"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+      </rPr>
+      <t>ModifyPartController</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">(){ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">throw new </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+      </rPr>
+      <t>UnsupportedOperationException(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+      </rPr>
+      <t>"Not implemented yet"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+      </rPr>
+      <t>}</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -261,6 +724,64 @@
       <family val="2"/>
       <charset val="238"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFA9B7C6"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF9876AA"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF6A8759"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC7832"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FFA9B7C6"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF9876AA"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFC66D"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="5">
@@ -362,7 +883,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -442,6 +963,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1068,7 +1598,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1112,8 +1642,12 @@
       <c r="H3" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
+      <c r="I3" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="J3" s="18">
+        <v>236</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="7" t="s">
@@ -1740,18 +2274,18 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="6"/>
     <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="18" style="6" customWidth="1"/>
-    <col min="5" max="5" width="24" style="6" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="55.7109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="61" style="6" customWidth="1"/>
+    <col min="6" max="6" width="97.42578125" style="6" customWidth="1"/>
     <col min="7" max="8" width="8.85546875" style="6"/>
     <col min="9" max="9" width="26.7109375" style="6" customWidth="1"/>
     <col min="10" max="16384" width="8.85546875" style="6"/>
@@ -1787,8 +2321,12 @@
       <c r="H3" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
+      <c r="I3" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="J3" s="18">
+        <v>236</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="17" t="s">
@@ -1843,210 +2381,258 @@
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="C10" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="38" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="C11" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="39" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C12" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="C13" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13" s="39" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="C14" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+      <c r="C15" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="F15" s="39" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="C28" s="1"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="C29" s="1"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="C30" s="1"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E31" s="11"/>
@@ -2057,7 +2643,9 @@
       </c>
       <c r="D32" s="37"/>
       <c r="E32" s="37"/>
-      <c r="F32" s="19"/>
+      <c r="F32" s="19">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -2068,6 +2656,7 @@
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="D6:E6"/>
   </mergeCells>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>